<commit_message>
Fix reference RIAA values
</commit_message>
<xml_diff>
--- a/lt1115-phono-mm-mc-v3/mesurements/RIAA-PreAmp-1.xlsx
+++ b/lt1115-phono-mm-mc-v3/mesurements/RIAA-PreAmp-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schenk/Documents/GitHub/electronic-projects/lt1115-phono-mm-mc-v3/mesurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCC30A3-AEF1-8D47-86A8-846F570864BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D83781-AC28-5F40-8D34-E62E92010112}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="480" windowWidth="28040" windowHeight="16500" activeTab="1" xr2:uid="{FC4D13F7-8D67-8143-BB8E-7AF9C7783FCE}"/>
   </bookViews>
@@ -2049,28 +2049,28 @@
                   <c:v>-1.5917235816989006E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-7.6211409228051252E-2</c:v>
+                  <c:v>-1.1186531065103367E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.17535127489629332</c:v>
+                  <c:v>-7.2452511466707392E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.29845223062358173</c:v>
+                  <c:v>-1.4467870786898374E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.54769394987676279</c:v>
+                  <c:v>-1.3916392250294507E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.71211855469453766</c:v>
+                  <c:v>-2.2753466670017986E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.0535516469653068</c:v>
+                  <c:v>6.2296399612016273E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.3282498319613545</c:v>
+                  <c:v>-3.9045502627317319E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-1.8536436118871507</c:v>
+                  <c:v>-2.0200038934037323E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>-1.5001996149342389E-2</c:v>
@@ -5449,8 +5449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB01C258-CB28-5443-A2E9-9219A72FD72E}">
   <dimension ref="A1:O86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+    <sheetView tabSelected="1" topLeftCell="L55" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5704,7 +5704,7 @@
         <v>75.238556768410575</v>
       </c>
       <c r="J11" s="18">
-        <v>18.895227403240199</v>
+        <v>18.830202525077251</v>
       </c>
       <c r="K11" s="18">
         <f t="shared" si="2"/>
@@ -5712,7 +5712,7 @@
       </c>
       <c r="L11" s="18">
         <f t="shared" si="3"/>
-        <v>-7.6211409228051252E-2</v>
+        <v>-1.1186531065103367E-2</v>
       </c>
       <c r="M11">
         <v>17.036986126710627</v>
@@ -5743,7 +5743,7 @@
         <v>74.979257225123234</v>
       </c>
       <c r="J12" s="18">
-        <v>18.7350677256211</v>
+        <v>18.566961701871477</v>
       </c>
       <c r="K12" s="18">
         <f t="shared" si="2"/>
@@ -5751,7 +5751,7 @@
       </c>
       <c r="L12" s="18">
         <f t="shared" si="3"/>
-        <v>-0.17535127489629332</v>
+        <v>-7.2452511466707392E-3</v>
       </c>
       <c r="M12">
         <v>17.093568184273323</v>
@@ -5782,7 +5782,7 @@
         <v>74.695996591776947</v>
       </c>
       <c r="J13" s="18">
-        <v>18.574908048002101</v>
+        <v>18.290923688165417</v>
       </c>
       <c r="K13" s="18">
         <f t="shared" si="2"/>
@@ -5790,7 +5790,7 @@
       </c>
       <c r="L13" s="18">
         <f t="shared" si="3"/>
-        <v>-0.29845223062358173</v>
+        <v>-1.4467870786898374E-2</v>
       </c>
       <c r="M13">
         <v>17.061666894853435</v>
@@ -5821,7 +5821,7 @@
         <v>74.286595194904663</v>
       </c>
       <c r="J14" s="18">
-        <v>18.414748370382998</v>
+        <v>17.88097081275653</v>
       </c>
       <c r="K14" s="18">
         <f t="shared" si="2"/>
@@ -5829,7 +5829,7 @@
       </c>
       <c r="L14" s="18">
         <f t="shared" si="3"/>
-        <v>-0.54769394987676279</v>
+        <v>-1.3916392250294507E-2</v>
       </c>
       <c r="M14">
         <v>16.91017733443331</v>
@@ -5860,7 +5860,7 @@
         <v>73.96201091246779</v>
       </c>
       <c r="J15" s="18">
-        <v>18.2545886927639</v>
+        <v>17.544745484736364</v>
       </c>
       <c r="K15" s="18">
         <f t="shared" si="2"/>
@@ -5868,7 +5868,7 @@
       </c>
       <c r="L15" s="18">
         <f t="shared" si="3"/>
-        <v>-0.71211855469453766</v>
+        <v>-2.2753466670017986E-3</v>
       </c>
       <c r="M15">
         <v>16.727620804952064</v>
@@ -5899,7 +5899,7 @@
         <v>73.460418142577922</v>
       </c>
       <c r="J16" s="18">
-        <v>18.094429015144801</v>
+        <v>17.034647728218292</v>
       </c>
       <c r="K16" s="18">
         <f t="shared" si="2"/>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="L16" s="18">
         <f t="shared" si="3"/>
-        <v>-1.0535516469653068</v>
+        <v>6.2296399612016273E-3</v>
       </c>
       <c r="M16">
         <v>16.388899938921416</v>
@@ -5938,7 +5938,7 @@
         <v>73.025560279962875</v>
       </c>
       <c r="J17" s="18">
-        <v>17.934269337525802</v>
+        <v>16.609924055827179</v>
       </c>
       <c r="K17" s="18">
         <f t="shared" si="2"/>
@@ -5946,7 +5946,7 @@
       </c>
       <c r="L17" s="18">
         <f t="shared" si="3"/>
-        <v>-1.3282498319613545</v>
+        <v>-3.9045502627317319E-3</v>
       </c>
       <c r="M17">
         <v>16.069583190732207</v>
@@ -5984,7 +5984,7 @@
         <v>72.340006822417976</v>
       </c>
       <c r="J18" s="18">
-        <v>17.774109659906699</v>
+        <v>15.940666086953586</v>
       </c>
       <c r="K18" s="18">
         <f t="shared" si="2"/>
@@ -5992,7 +5992,7 @@
       </c>
       <c r="L18" s="18">
         <f t="shared" si="3"/>
-        <v>-1.8536436118871507</v>
+        <v>-2.0200038934037323E-2</v>
       </c>
       <c r="M18">
         <v>15.522881381848732</v>
@@ -8631,7 +8631,7 @@
   <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C83"/>
+      <selection activeCell="B5" sqref="B5:B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>